<commit_message>
Added test case data for FSF
</commit_message>
<xml_diff>
--- a/SOFL/ProcessFunctionalScenariosandTestCases.xlsx
+++ b/SOFL/ProcessFunctionalScenariosandTestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeka/projects/salon_booking/salon_api/SOFL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41491B49-8DAD-CA4A-9F68-0353C43CA9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA19C3A-1305-3148-B6D3-6AE42DE4A5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{F7442594-F3B3-1741-80EA-B662262E1679}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F7442594-F3B3-1741-80EA-B662262E1679}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="155">
   <si>
     <t>Process Specification</t>
   </si>
@@ -46,9 +44,6 @@
   </si>
   <si>
     <t>Expected Results</t>
-  </si>
-  <si>
-    <t>Execution Results</t>
   </si>
   <si>
     <t>RetrieveSalon</t>
@@ -246,13 +241,271 @@
   </si>
   <si>
     <t>error_message = "Http 403, Forbidden" =&gt; len(access_token) &lt;&gt; 0 and access_token &lt;&gt; nil and exists![i: inset dom(~salon_customers_table)] | i.id = customer_id | salon_customers_table(i) = salon | i.role &lt;&gt; &lt;SALONCUSTOMER&gt;</t>
+  </si>
+  <si>
+    <t>GetSalonBookings</t>
+  </si>
+  <si>
+    <t>bookings = salon_bookings_table =&gt;len(access_token) &lt;&gt; 0 and access_token &lt;&gt; nil exists[i: inset dom(salon_bookings_table)] | salon_bookings_table(i) = user and user.role = &lt;SALONCUSTOMER&gt; and response_status = "Http 200"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error_message = "Http 401, Permission Denied" =&gt; len(access_token) = 0 and user.role = &lt;SALONCUSTOMER&gt; </t>
+  </si>
+  <si>
+    <t>error_message = "Http 403, Forbidden" =&gt; len(access_token) &lt;&gt; 0 and access_token &lt;&gt; nil exists[i: inset dom(salon_bookings_table)] | salon_bookings_table(i) = user | salon_bookings_table(i).role &lt;&gt; &lt;SALONCUSTOMER&gt;</t>
+  </si>
+  <si>
+    <t>GetSalonBooking</t>
+  </si>
+  <si>
+    <t>exists![i: inset dom(salon_bookings_table)] | i.id = booking_id and booking.id = booking_id | salon_bookings_table(i) = user =&gt; len(access_token) &lt;&gt; 0 and access_token &lt;&gt; nil and booking inset dom(salon_bookings_table) and salon_bookings_table(booking) = user and salon_bookings_table(boooking).role = &lt;SALONCUSTOMER&gt; and response_status = "Http 200 Ok"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> error_message = "Http 401, Permission Denied" =&gt; len(access_token) = 0 and exists![i: inset dom(salon_bookings_table)] | i.id = booking_id | salon_bookings_table(i) = user and user.role = &lt;SALONCSUTOMER&gt;</t>
+  </si>
+  <si>
+    <t>error_message = "Http 401, Permission Denied"=&gt; access_token = nil and exists![i: inset dom(salon_bookings_table)] | i.id = booking_id | salon_bookings_table(i) = user and user.role = &lt;SALONCSUTOMER&gt;</t>
+  </si>
+  <si>
+    <t>error_message ="Http 403, Forbidden" =&gt; len(access_token) &lt;&gt; 0 and access_token &lt;&gt; nil and exists![i: inset dom(salon_bookings_table)] | i.id = booking_id | salon_bookings_table(i) = user and user.role &lt;&gt; &lt;SALONCSUTOMER&gt;</t>
+  </si>
+  <si>
+    <t>DeleteSalonBooking</t>
+  </si>
+  <si>
+    <t>salon_bookings_table = override(~salon_bookings_table, {deleted_booking -&gt; user}) and user.role = &lt;SALONOWNER&gt; =&gt; len(access_token) &lt;&gt; 0 and access_token &lt;&gt; nil and exists![i: inset dom(salon_bookings_table)] | i.id = booking_id | salon_bookings_table(i) = user and salon_bookings_table(deleted_booking) = user and user.role = &lt;SALONCUSTOMER&gt; and response_status = "Http 204"</t>
+  </si>
+  <si>
+    <t>error_message = "Http 401, Permission Denied" =&gt; len(access_token) = 0 and exists[i: inset dom(salon_bookings_table)] | i.id = booking_id | salon_bookings_table(i) = user and user.role = &lt;SALONOWNER&gt;</t>
+  </si>
+  <si>
+    <t>error_message = "Http 401, Permission Denied" =&gt; access_token = nil and exists![i: inset dom(salon_bookings_table)] | i.id = booking_id | salon_bookings_table(i) = user and user.role = &lt;SALONOWNER&gt;</t>
+  </si>
+  <si>
+    <t>error_message = "Http 403, Forbidden" =&gt; len(access_token) &lt;&gt; 0  and access_token &lt;&gt; nil and exists![i: inset dom(salon_bookings_table)] | i.id = booking_id | salon_bookings_table(i) = user and salon_bookings_table(deleted_booking) = user and user.role &lt;&gt; &lt;SALONCUSTOMER&gt;</t>
+  </si>
+  <si>
+    <t>Http 200</t>
+  </si>
+  <si>
+    <t>("XVfT345", "uuid_34567", salonuser)</t>
+  </si>
+  <si>
+    <t>(" ", "uuid_34567", salonuser)</t>
+  </si>
+  <si>
+    <t>("nil", "uuid_34567", salonuser)</t>
+  </si>
+  <si>
+    <t>Test Case notes</t>
+  </si>
+  <si>
+    <t>salonuser.role == &lt;SALONOWNER&gt;</t>
+  </si>
+  <si>
+    <t>salonuser.role != &lt;SALONOWNER&gt;</t>
+  </si>
+  <si>
+    <t>Http 401</t>
+  </si>
+  <si>
+    <t>"Execution" Results</t>
+  </si>
+  <si>
+    <t>Http 403</t>
+  </si>
+  <si>
+    <t>("XVFT456ty", '/salons')</t>
+  </si>
+  <si>
+    <t>(" ", '/salons')</t>
+  </si>
+  <si>
+    <t>(nil, '/salons')</t>
+  </si>
+  <si>
+    <t>Htttp 401</t>
+  </si>
+  <si>
+    <t>("XVfT345", "uuid_34567_778", salon, owner)</t>
+  </si>
+  <si>
+    <t>owner.role == &lt;SALONOWNER&gt;</t>
+  </si>
+  <si>
+    <t>(" ", "uuid_34567_778", salon, owner)</t>
+  </si>
+  <si>
+    <t>(nil, "uuid_34567_778", salon, owner)</t>
+  </si>
+  <si>
+    <t>owner.role != &lt;SALONOWNER&gt;</t>
+  </si>
+  <si>
+    <t>("ZXvFT345", "uuid_34567_778",  owner)</t>
+  </si>
+  <si>
+    <t>(nil, "uuid_34567_778",  owner)</t>
+  </si>
+  <si>
+    <t>(" ", "uuid_34567_778",  owner)</t>
+  </si>
+  <si>
+    <t>Http 204</t>
+  </si>
+  <si>
+    <t>("ZXvFT345", category)</t>
+  </si>
+  <si>
+    <t>Http 200 Ok</t>
+  </si>
+  <si>
+    <t>(" ", category)</t>
+  </si>
+  <si>
+    <t>(nil, category)</t>
+  </si>
+  <si>
+    <t>("XcVFt678", "uuid_cat_789")</t>
+  </si>
+  <si>
+    <t>(" ", "uuid_cat_789")</t>
+  </si>
+  <si>
+    <t>(nil, "uuid_cat_789")</t>
+  </si>
+  <si>
+    <t>("XcVFt678", "uuid_456_sal", "uuid_cat_789")</t>
+  </si>
+  <si>
+    <t>(" ", "uuid_456_sal", "uuid_cat_789")</t>
+  </si>
+  <si>
+    <t>(nil, "uuid_456_sal", "uuid_cat_789")</t>
+  </si>
+  <si>
+    <t>("XcVFt678",  user, category)</t>
+  </si>
+  <si>
+    <t>user.role ==  &lt;SALONOWNER&gt;</t>
+  </si>
+  <si>
+    <t>(" ",  user, category)</t>
+  </si>
+  <si>
+    <t>(nil,  user, category)</t>
+  </si>
+  <si>
+    <t>user.role !=  &lt;SALONOWNER&gt;</t>
+  </si>
+  <si>
+    <t>("Xsdfrt56", salon, "uuid_457", salonuser)</t>
+  </si>
+  <si>
+    <t>error_message = "Http 401, Permission Denied" =&gt; access_token = nil and salons_table(salon) = salonuser and salonuser.role = &lt;SALONOWNER&gt; and error_message = "Http 401, Permission Denied"</t>
+  </si>
+  <si>
+    <t>(" ", salon, "uuid_457", salonuser)</t>
+  </si>
+  <si>
+    <t>nil, salon, "uuid_457", salonuser)</t>
+  </si>
+  <si>
+    <t>error_message = "Http 401, Permission Denied" =&gt; access_token = nil and salons_table(salon) = salonuser and salonuser.role = &lt;SALONOWNER&gt;</t>
+  </si>
+  <si>
+    <t>Http. 403</t>
+  </si>
+  <si>
+    <t>(nil, salon, "uuid_457", salonuser)</t>
+  </si>
+  <si>
+    <t>("Xsdfrt56", salon, salonuser, saloncustomer)</t>
+  </si>
+  <si>
+    <t>(" ", salon, salonuser, saloncustomer)</t>
+  </si>
+  <si>
+    <t>(nil, salon, salonuser, saloncustomer)</t>
+  </si>
+  <si>
+    <t>("Xsdfrt56", "uuid_salo_xzf", "uuid_457_cust_er34" )</t>
+  </si>
+  <si>
+    <t>(" ", "uuid_salo_xzf", "uuid_457_cust_er34" )</t>
+  </si>
+  <si>
+    <t>(nil, "uuid_salo_xzf", "uuid_457_cust_er34" )</t>
+  </si>
+  <si>
+    <t>customer.role  != &lt;SALONCUSTOMER&gt;</t>
+  </si>
+  <si>
+    <t>customer.role  == &lt;SALONCUSTOMER&gt;</t>
+  </si>
+  <si>
+    <t>salonuser.role  == &lt;SALONCUSTOMER&gt;</t>
+  </si>
+  <si>
+    <t>salonuser.role  != &lt;SALONCUSTOMER&gt;</t>
+  </si>
+  <si>
+    <t>GetSalonCustomer</t>
+  </si>
+  <si>
+    <t>("Xsdfrt56", salon, salonuser, saloncustomer )</t>
+  </si>
+  <si>
+    <t>(" ", salon, salonuser, saloncustomer )</t>
+  </si>
+  <si>
+    <t>("XvF567ty", salon, "uuid_cust_678")</t>
+  </si>
+  <si>
+    <t>(" ", salon, "uuid_cust_678")</t>
+  </si>
+  <si>
+    <t>(nil, salon, "uuid_cust_678")</t>
+  </si>
+  <si>
+    <t>("Xvfrty567", user)</t>
+  </si>
+  <si>
+    <t>user.role != &lt;SALONCUSTOMER&gt;</t>
+  </si>
+  <si>
+    <t>(nil, user)</t>
+  </si>
+  <si>
+    <t>(" ", user)</t>
+  </si>
+  <si>
+    <t>user.role == &lt;SALONCUSTOMER&gt;</t>
+  </si>
+  <si>
+    <t>Http 200 ok</t>
+  </si>
+  <si>
+    <t>("XvF45678", user, "uuid_booking_567"</t>
+  </si>
+  <si>
+    <t>(nil, user, "uuid_booking_567"</t>
+  </si>
+  <si>
+    <t>(" ", user, "uuid_booking_567"</t>
+  </si>
+  <si>
+    <t>user.role != &lt;SALONOWNER&gt;</t>
+  </si>
+  <si>
+    <t>user.role == &lt;SALONOWNER&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -264,6 +517,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -289,14 +549,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,22 +872,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317A6751-6D5B-1C45-91EE-81F1761D2D6F}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58.5" customWidth="1"/>
-    <col min="2" max="2" width="63.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="65.83203125" customWidth="1"/>
+    <col min="3" max="3" width="48.83203125" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" customWidth="1"/>
+    <col min="5" max="5" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -637,401 +899,1235 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="82" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="119" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="119" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="1" t="s">
+      <c r="C10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="62" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="113" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="113" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="88" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="88" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="B20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="118" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="B23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="106" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="106" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="B26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="151" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="151" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="B29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" t="s">
+        <v>107</v>
+      </c>
+      <c r="F29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="B30" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E30" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="76" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="76" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="B33" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" s="1" t="s">
+      <c r="C36" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="B37" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" t="s">
+        <v>107</v>
+      </c>
+      <c r="F37" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" t="s">
+        <v>90</v>
+      </c>
+      <c r="F38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
+      <c r="B39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" t="s">
+        <v>88</v>
+      </c>
+      <c r="E39" t="s">
+        <v>90</v>
+      </c>
+      <c r="F39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D40" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" t="s">
+        <v>126</v>
+      </c>
+      <c r="F40" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+      <c r="B41" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C41" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" t="s">
+        <v>88</v>
+      </c>
+      <c r="E41" t="s">
+        <v>107</v>
+      </c>
+      <c r="F41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3"/>
+      <c r="B42" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="1" t="s">
+      <c r="C42" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" t="s">
+        <v>90</v>
+      </c>
+      <c r="F42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="B43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D43" t="s">
+        <v>88</v>
+      </c>
+      <c r="E43" t="s">
+        <v>90</v>
+      </c>
+      <c r="F43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="B44" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="1" t="s">
+      <c r="C44" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D44" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="124" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="124" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+      <c r="B45" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C45" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D45" t="s">
+        <v>136</v>
+      </c>
+      <c r="E45" t="s">
+        <v>107</v>
+      </c>
+      <c r="F45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="89" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
+      <c r="B46" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="89" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="1" t="s">
+      <c r="C46" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D46" t="s">
+        <v>136</v>
+      </c>
+      <c r="E46" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="91" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="91" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="1" t="s">
+      <c r="C47" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" t="s">
+        <v>136</v>
+      </c>
+      <c r="E47" t="s">
+        <v>90</v>
+      </c>
+      <c r="F47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="4"/>
+      <c r="B48" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="B45" s="1" t="s">
+      <c r="C48" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" t="s">
+        <v>137</v>
+      </c>
+      <c r="E48" t="s">
+        <v>92</v>
+      </c>
+      <c r="F48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="124" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C49" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D49" t="s">
+        <v>135</v>
+      </c>
+      <c r="E49" t="s">
+        <v>107</v>
+      </c>
+      <c r="F49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" t="s">
+        <v>135</v>
+      </c>
+      <c r="E50" t="s">
+        <v>90</v>
+      </c>
+      <c r="F50" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D51" t="s">
+        <v>135</v>
+      </c>
+      <c r="E51" t="s">
+        <v>90</v>
+      </c>
+      <c r="F51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+      <c r="B52" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D52" t="s">
+        <v>134</v>
+      </c>
+      <c r="E52" t="s">
+        <v>92</v>
+      </c>
+      <c r="F52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="124" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D53" t="s">
+        <v>135</v>
+      </c>
+      <c r="E53" t="s">
+        <v>107</v>
+      </c>
+      <c r="F53" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="4"/>
+      <c r="B54" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D54" t="s">
+        <v>135</v>
+      </c>
+      <c r="E54" t="s">
+        <v>90</v>
+      </c>
+      <c r="F54" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="4"/>
+      <c r="B55" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="1" t="s">
+      <c r="C55" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D55" t="s">
+        <v>135</v>
+      </c>
+      <c r="E55" t="s">
+        <v>90</v>
+      </c>
+      <c r="F55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+      <c r="B56" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
-      <c r="B52" s="1" t="s">
+      <c r="C56" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D56" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" t="s">
+        <v>92</v>
+      </c>
+      <c r="F56" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="1:2" ht="79" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="1"/>
-    </row>
-    <row r="55" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="1"/>
-    </row>
-    <row r="56" spans="1:2" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="1:2" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="1"/>
-    </row>
-    <row r="58" spans="1:2" ht="77" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="1"/>
-    </row>
-    <row r="59" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="1:2" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="1:2" ht="61" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="1:2" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="1"/>
-    </row>
-    <row r="63" spans="1:2" ht="71" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="1"/>
-    </row>
-    <row r="64" spans="1:2" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="1"/>
+      <c r="B57" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D57" t="s">
+        <v>148</v>
+      </c>
+      <c r="E57" t="s">
+        <v>149</v>
+      </c>
+      <c r="F57" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="3"/>
+      <c r="B58" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D58" t="s">
+        <v>148</v>
+      </c>
+      <c r="E58" t="s">
+        <v>90</v>
+      </c>
+      <c r="F58" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="3"/>
+      <c r="B59" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D59" t="s">
+        <v>148</v>
+      </c>
+      <c r="E59" t="s">
+        <v>90</v>
+      </c>
+      <c r="F59" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="B60" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D60" t="s">
+        <v>145</v>
+      </c>
+      <c r="E60" t="s">
+        <v>92</v>
+      </c>
+      <c r="F60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D61" t="s">
+        <v>148</v>
+      </c>
+      <c r="E61" t="s">
+        <v>107</v>
+      </c>
+      <c r="F61" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="3"/>
+      <c r="B62" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D62" t="s">
+        <v>148</v>
+      </c>
+      <c r="E62" t="s">
+        <v>90</v>
+      </c>
+      <c r="F62" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="77" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="3"/>
+      <c r="B63" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D63" t="s">
+        <v>148</v>
+      </c>
+      <c r="E63" t="s">
+        <v>90</v>
+      </c>
+      <c r="F63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="3"/>
+      <c r="B64" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D64" t="s">
+        <v>145</v>
+      </c>
+      <c r="E64" t="s">
+        <v>92</v>
+      </c>
+      <c r="F64" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="115" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D65" t="s">
+        <v>154</v>
+      </c>
+      <c r="E65" t="s">
+        <v>107</v>
+      </c>
+      <c r="F65" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="3"/>
+      <c r="B66" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D66" t="s">
+        <v>154</v>
+      </c>
+      <c r="E66" t="s">
+        <v>90</v>
+      </c>
+      <c r="F66" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="3"/>
+      <c r="B67" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D67" t="s">
+        <v>154</v>
+      </c>
+      <c r="E67" t="s">
+        <v>90</v>
+      </c>
+      <c r="F67" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="3"/>
+      <c r="B68" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D68" t="s">
+        <v>153</v>
+      </c>
+      <c r="E68" t="s">
+        <v>92</v>
+      </c>
+      <c r="F68" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A39:A41"/>
+  <mergeCells count="18">
+    <mergeCell ref="A20:A22"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A61:A64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>